<commit_message>
Fix: bind to correct port for Render
</commit_message>
<xml_diff>
--- a/backend/exports/1/dummy_excel_data.xlsx
+++ b/backend/exports/1/dummy_excel_data.xlsx
@@ -538,12 +538,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>데이터A★</t>
+          <t>데이터A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>데이터A</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>데이터C</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>데이터C</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>데이터B</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>데이터C</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1456,7 +1456,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>데이터C★</t>
+          <t>데이터C</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2068,7 +2068,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>데이터C★</t>
+          <t>데이터C</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2374,7 +2374,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>데이터E★</t>
+          <t>데이터E</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>데이터B</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>데이터E</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2986,7 +2986,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>데이터C★</t>
+          <t>데이터C</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3088,7 +3088,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>데이터E★</t>
+          <t>데이터E</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3399,7 +3399,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>데이터D</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>데이터C</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -3603,7 +3603,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>데이터D</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -3700,7 +3700,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>데이터C★</t>
+          <t>데이터C</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3904,7 +3904,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>데이터E★</t>
+          <t>데이터E</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -4215,7 +4215,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>데이터D</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -4618,7 +4618,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>데이터C★</t>
+          <t>데이터C</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -4720,7 +4720,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>데이터E★</t>
+          <t>데이터E</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>데이터C</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -5031,7 +5031,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>데이터B</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -5332,7 +5332,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>데이터D★</t>
+          <t>데이터D</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">

</xml_diff>